<commit_message>
Edit studentofficial.xlsx, add grade.xlsx, add course.xlsx, fix traningcenterframe
</commit_message>
<xml_diff>
--- a/studentofficial.xlsx
+++ b/studentofficial.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaProject\StudentManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\StudentManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35FCC084-FEE9-444D-B796-2327AF652E6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F00C79A-040D-48E3-8642-78B1C79A962A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7807A4F5-D986-42A2-AF98-174C4FA974EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7807A4F5-D986-42A2-AF98-174C4FA974EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -406,6 +406,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -721,15 +722,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9A2BE2-4B75-4C9C-B474-79CA86735FCE}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K27"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="39.75" thickBot="1">
+    <row r="1" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A1" s="1">
         <v>102180171</v>
       </c>
@@ -763,8 +764,23 @@
       <c r="K1" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L1" s="17">
+        <v>8</v>
+      </c>
+      <c r="M1" s="17">
+        <v>9</v>
+      </c>
+      <c r="N1" s="17">
+        <v>0</v>
+      </c>
+      <c r="O1" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="P1" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A2" s="9">
         <v>102180009</v>
       </c>
@@ -798,8 +814,23 @@
       <c r="K2" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L2" s="17">
+        <v>9</v>
+      </c>
+      <c r="M2" s="17">
+        <v>7</v>
+      </c>
+      <c r="N2" s="17">
+        <v>-3</v>
+      </c>
+      <c r="O2" s="17">
+        <v>2000000</v>
+      </c>
+      <c r="P2" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="54" thickBot="1">
       <c r="A3" s="1">
         <v>102180021</v>
       </c>
@@ -833,8 +864,23 @@
       <c r="K3" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L3" s="17">
+        <v>8</v>
+      </c>
+      <c r="M3" s="17">
+        <v>8.5</v>
+      </c>
+      <c r="N3" s="17">
+        <v>0</v>
+      </c>
+      <c r="O3" s="17">
+        <v>1200000</v>
+      </c>
+      <c r="P3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="54" thickBot="1">
       <c r="A4" s="9">
         <v>102180101</v>
       </c>
@@ -868,8 +914,23 @@
       <c r="K4" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L4" s="17">
+        <v>8</v>
+      </c>
+      <c r="M4" s="17">
+        <v>7</v>
+      </c>
+      <c r="N4" s="17">
+        <v>0</v>
+      </c>
+      <c r="O4" s="17">
+        <v>500000</v>
+      </c>
+      <c r="P4" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="54" thickBot="1">
       <c r="A5" s="1">
         <v>102180005</v>
       </c>
@@ -903,8 +964,23 @@
       <c r="K5" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L5" s="17">
+        <v>6</v>
+      </c>
+      <c r="M5" s="17">
+        <v>8</v>
+      </c>
+      <c r="N5" s="17">
+        <v>0</v>
+      </c>
+      <c r="O5" s="17">
+        <v>100000</v>
+      </c>
+      <c r="P5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A6" s="9">
         <v>102180180</v>
       </c>
@@ -938,8 +1014,23 @@
       <c r="K6" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L6" s="17">
+        <v>7</v>
+      </c>
+      <c r="M6" s="17">
+        <v>9</v>
+      </c>
+      <c r="N6" s="17">
+        <v>0</v>
+      </c>
+      <c r="O6" s="17">
+        <v>2000000</v>
+      </c>
+      <c r="P6" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A7" s="1">
         <v>102180035</v>
       </c>
@@ -973,8 +1064,23 @@
       <c r="K7" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="58.5" thickBot="1">
+      <c r="L7" s="17">
+        <v>8</v>
+      </c>
+      <c r="M7" s="17">
+        <v>9.5</v>
+      </c>
+      <c r="N7" s="17">
+        <v>-2</v>
+      </c>
+      <c r="O7" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="P7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="56.4" thickBot="1">
       <c r="A8" s="9">
         <v>102180069</v>
       </c>
@@ -1008,8 +1114,23 @@
       <c r="K8" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L8" s="17">
+        <v>9</v>
+      </c>
+      <c r="M8" s="17">
+        <v>6</v>
+      </c>
+      <c r="N8" s="17">
+        <v>0</v>
+      </c>
+      <c r="O8" s="17">
+        <v>2500000</v>
+      </c>
+      <c r="P8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A9" s="1">
         <v>102180103</v>
       </c>
@@ -1043,8 +1164,23 @@
       <c r="K9" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L9" s="17">
+        <v>5</v>
+      </c>
+      <c r="M9" s="17">
+        <v>7</v>
+      </c>
+      <c r="N9" s="17">
+        <v>0</v>
+      </c>
+      <c r="O9" s="17">
+        <v>0</v>
+      </c>
+      <c r="P9" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A10" s="9">
         <v>102180003</v>
       </c>
@@ -1078,8 +1214,23 @@
       <c r="K10" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L10" s="17">
+        <v>6</v>
+      </c>
+      <c r="M10" s="17">
+        <v>9</v>
+      </c>
+      <c r="N10" s="17">
+        <v>0</v>
+      </c>
+      <c r="O10" s="17">
+        <v>1200000</v>
+      </c>
+      <c r="P10" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A11" s="1">
         <v>102180108</v>
       </c>
@@ -1113,8 +1264,23 @@
       <c r="K11" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L11" s="17">
+        <v>4</v>
+      </c>
+      <c r="M11" s="17">
+        <v>9</v>
+      </c>
+      <c r="N11" s="17">
+        <v>0</v>
+      </c>
+      <c r="O11" s="17">
+        <v>0</v>
+      </c>
+      <c r="P11" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="54" thickBot="1">
       <c r="A12" s="9">
         <v>102180232</v>
       </c>
@@ -1148,8 +1314,23 @@
       <c r="K12" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L12" s="17">
+        <v>9</v>
+      </c>
+      <c r="M12" s="17">
+        <v>7.5</v>
+      </c>
+      <c r="N12" s="17">
+        <v>-5</v>
+      </c>
+      <c r="O12" s="17">
+        <v>0</v>
+      </c>
+      <c r="P12" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A13" s="1">
         <v>102180013</v>
       </c>
@@ -1183,8 +1364,23 @@
       <c r="K13" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L13" s="17">
+        <v>9</v>
+      </c>
+      <c r="M13" s="17">
+        <v>8.5</v>
+      </c>
+      <c r="N13" s="17">
+        <v>-1</v>
+      </c>
+      <c r="O13" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="P13" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A14" s="9">
         <v>102180041</v>
       </c>
@@ -1218,8 +1414,23 @@
       <c r="K14" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L14" s="17">
+        <v>10</v>
+      </c>
+      <c r="M14" s="17">
+        <v>8</v>
+      </c>
+      <c r="N14" s="17">
+        <v>0</v>
+      </c>
+      <c r="O14" s="17">
+        <v>2000000</v>
+      </c>
+      <c r="P14" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A15" s="1">
         <v>102180177</v>
       </c>
@@ -1253,8 +1464,23 @@
       <c r="K15" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L15" s="17">
+        <v>9</v>
+      </c>
+      <c r="M15" s="17">
+        <v>8</v>
+      </c>
+      <c r="N15" s="17">
+        <v>-5</v>
+      </c>
+      <c r="O15" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="P15" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A16" s="9">
         <v>102180214</v>
       </c>
@@ -1288,8 +1514,23 @@
       <c r="K16" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L16" s="17">
+        <v>8</v>
+      </c>
+      <c r="M16" s="17">
+        <v>7.5</v>
+      </c>
+      <c r="N16" s="17">
+        <v>-4</v>
+      </c>
+      <c r="O16" s="17">
+        <v>2000000</v>
+      </c>
+      <c r="P16" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="67.2" thickBot="1">
       <c r="A17" s="1">
         <v>102180256</v>
       </c>
@@ -1323,8 +1564,23 @@
       <c r="K17" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L17" s="17">
+        <v>7.5</v>
+      </c>
+      <c r="M17" s="17">
+        <v>9</v>
+      </c>
+      <c r="N17" s="17">
+        <v>0</v>
+      </c>
+      <c r="O17" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="P17" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A18" s="9">
         <v>102180250</v>
       </c>
@@ -1358,8 +1614,23 @@
       <c r="K18" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L18" s="17">
+        <v>9.5</v>
+      </c>
+      <c r="M18" s="17">
+        <v>9</v>
+      </c>
+      <c r="N18" s="17">
+        <v>0</v>
+      </c>
+      <c r="O18" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="P18" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A19" s="1">
         <v>102180207</v>
       </c>
@@ -1393,8 +1664,23 @@
       <c r="K19" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L19" s="17">
+        <v>6.5</v>
+      </c>
+      <c r="M19" s="17">
+        <v>9</v>
+      </c>
+      <c r="N19" s="17">
+        <v>-1</v>
+      </c>
+      <c r="O19" s="17">
+        <v>500000</v>
+      </c>
+      <c r="P19" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="54" thickBot="1">
       <c r="A20" s="9">
         <v>102180174</v>
       </c>
@@ -1428,8 +1714,23 @@
       <c r="K20" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L20" s="17">
+        <v>8.5</v>
+      </c>
+      <c r="M20" s="17">
+        <v>10</v>
+      </c>
+      <c r="N20" s="17">
+        <v>-1</v>
+      </c>
+      <c r="O20" s="17">
+        <v>2100000</v>
+      </c>
+      <c r="P20" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="54" thickBot="1">
       <c r="A21" s="1">
         <v>102180001</v>
       </c>
@@ -1463,8 +1764,23 @@
       <c r="K21" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L21" s="17">
+        <v>7</v>
+      </c>
+      <c r="M21" s="17">
+        <v>10</v>
+      </c>
+      <c r="N21" s="17">
+        <v>0</v>
+      </c>
+      <c r="O21" s="17">
+        <v>0</v>
+      </c>
+      <c r="P21" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A22" s="9">
         <v>102180064</v>
       </c>
@@ -1498,8 +1814,23 @@
       <c r="K22" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L22" s="17">
+        <v>7</v>
+      </c>
+      <c r="M22" s="17">
+        <v>10</v>
+      </c>
+      <c r="N22" s="17">
+        <v>0</v>
+      </c>
+      <c r="O22" s="17">
+        <v>0</v>
+      </c>
+      <c r="P22" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="54" thickBot="1">
       <c r="A23" s="1">
         <v>102180149</v>
       </c>
@@ -1533,8 +1864,23 @@
       <c r="K23" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L23" s="17">
+        <v>9.5</v>
+      </c>
+      <c r="M23" s="17">
+        <v>8.5</v>
+      </c>
+      <c r="N23" s="17">
+        <v>-2</v>
+      </c>
+      <c r="O23" s="17">
+        <v>1500000</v>
+      </c>
+      <c r="P23" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A24" s="9">
         <v>102180248</v>
       </c>
@@ -1568,8 +1914,23 @@
       <c r="K24" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L24" s="17">
+        <v>9</v>
+      </c>
+      <c r="M24" s="17">
+        <v>8</v>
+      </c>
+      <c r="N24" s="17">
+        <v>-3</v>
+      </c>
+      <c r="O24" s="17">
+        <v>0</v>
+      </c>
+      <c r="P24" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="54" thickBot="1">
       <c r="A25" s="1">
         <v>102180033</v>
       </c>
@@ -1603,8 +1964,23 @@
       <c r="K25" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="52.5" thickBot="1">
+      <c r="L25" s="17">
+        <v>9</v>
+      </c>
+      <c r="M25" s="17">
+        <v>9</v>
+      </c>
+      <c r="N25" s="17">
+        <v>-4</v>
+      </c>
+      <c r="O25" s="17">
+        <v>0</v>
+      </c>
+      <c r="P25" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="54" thickBot="1">
       <c r="A26" s="9">
         <v>102180061</v>
       </c>
@@ -1638,8 +2014,23 @@
       <c r="K26" s="7">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="39.75" thickBot="1">
+      <c r="L26" s="17">
+        <v>10</v>
+      </c>
+      <c r="M26" s="17">
+        <v>9</v>
+      </c>
+      <c r="N26" s="17">
+        <v>0</v>
+      </c>
+      <c r="O26" s="17">
+        <v>2000000</v>
+      </c>
+      <c r="P26" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="40.799999999999997" thickBot="1">
       <c r="A27" s="1">
         <v>102180224</v>
       </c>
@@ -1672,6 +2063,21 @@
       </c>
       <c r="K27" s="7">
         <v>4000000</v>
+      </c>
+      <c r="L27" s="17">
+        <v>6</v>
+      </c>
+      <c r="M27" s="17">
+        <v>8</v>
+      </c>
+      <c r="N27" s="17">
+        <v>0</v>
+      </c>
+      <c r="O27" s="17">
+        <v>1500000</v>
+      </c>
+      <c r="P27" s="17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>